<commit_message>
- Added a spreadsheet for tiles at leve.
</commit_message>
<xml_diff>
--- a/TilesAtLevel.xlsx
+++ b/TilesAtLevel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Level</t>
   </si>
@@ -29,6 +29,24 @@
   <si>
     <t>Number</t>
   </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
+  </si>
+  <si>
+    <t>Tiles per second</t>
+  </si>
+  <si>
+    <t>Duration S</t>
+  </si>
+  <si>
+    <t>Cumulative Tiles</t>
+  </si>
+  <si>
+    <t>Duration Hours</t>
+  </si>
 </sst>
 </file>
 
@@ -36,7 +54,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -75,9 +93,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -359,19 +379,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +404,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -394,8 +423,16 @@
         <f>B2*B2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <f>C2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <f>D2/(3600*G$6)</f>
+        <v>3.4722222222222222E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -407,8 +444,22 @@
         <f t="shared" ref="C3:C20" si="1">B3*B3</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <f>C3+D2</f>
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3/(3600*G$6)</f>
+        <v>1.7361111111111112E-4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -420,8 +471,22 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D20" si="2">C4+D3</f>
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E20" si="3">D4/(3600*G$6)</f>
+        <v>7.291666666666667E-4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -433,8 +498,23 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="3"/>
+        <v>2.9513888888888888E-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <f>3600*1.5</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -446,8 +526,22 @@
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f t="shared" si="2"/>
+        <v>341</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1840277777777778E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -459,8 +553,20 @@
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f t="shared" si="2"/>
+        <v>1365</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="3"/>
+        <v>4.7395833333333331E-2</v>
+      </c>
+      <c r="G7">
+        <f>7*3600</f>
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -472,8 +578,16 @@
         <f t="shared" si="1"/>
         <v>4096</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" si="2"/>
+        <v>5461</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.18961805555555555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -485,8 +599,16 @@
         <f t="shared" si="1"/>
         <v>16384</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f t="shared" si="2"/>
+        <v>21845</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.75850694444444444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -498,8 +620,16 @@
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="2"/>
+        <v>87381</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="3"/>
+        <v>3.0340625000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -511,8 +641,16 @@
         <f t="shared" si="1"/>
         <v>262144</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="2"/>
+        <v>349525</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="3"/>
+        <v>12.136284722222221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -524,8 +662,16 @@
         <f t="shared" si="1"/>
         <v>1048576</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="2"/>
+        <v>1398101</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="3"/>
+        <v>48.54517361111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -537,8 +683,16 @@
         <f t="shared" si="1"/>
         <v>4194304</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="2"/>
+        <v>5592405</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="3"/>
+        <v>194.18072916666668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -550,8 +704,16 @@
         <f t="shared" si="1"/>
         <v>16777216</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="2"/>
+        <v>22369621</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="3"/>
+        <v>776.72295138888887</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -563,8 +725,16 @@
         <f t="shared" si="1"/>
         <v>67108864</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="2"/>
+        <v>89478485</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>3106.8918402777776</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -576,8 +746,16 @@
         <f t="shared" si="1"/>
         <v>268435456</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="2"/>
+        <v>357913941</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="3"/>
+        <v>12427.567395833334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -589,8 +767,16 @@
         <f t="shared" si="1"/>
         <v>1073741824</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="2"/>
+        <v>1431655765</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="3"/>
+        <v>49710.269618055558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -602,8 +788,16 @@
         <f t="shared" si="1"/>
         <v>4294967296</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="2"/>
+        <v>5726623061</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="3"/>
+        <v>198841.07850694444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -615,8 +809,16 @@
         <f t="shared" si="1"/>
         <v>17179869184</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="2"/>
+        <v>22906492245</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="3"/>
+        <v>795364.31406250002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -627,6 +829,14 @@
       <c r="C20" s="1">
         <f t="shared" si="1"/>
         <v>68719476736</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="2"/>
+        <v>91625968981</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="3"/>
+        <v>3181457.2562847221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>